<commit_message>
Some serial - home missing, but overall all tests completed
</commit_message>
<xml_diff>
--- a/AllResults_Table - runs.xlsx
+++ b/AllResults_Table - runs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete Table Of Results" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>ALL RESULTS</t>
   </si>
@@ -97,6 +97,12 @@
   <si>
     <t>Serial - no technique applied</t>
   </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Serial Algorithms</t>
+  </si>
 </sst>
 </file>
 
@@ -107,7 +113,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +290,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -470,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -716,6 +730,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -768,7 +824,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="9" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1"/>
@@ -801,6 +857,17 @@
     <xf numFmtId="0" fontId="16" fillId="18" borderId="11" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="18" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -831,26 +898,35 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1203,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1225,49 +1301,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="26"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="37"/>
       <c r="P1" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
     </row>
     <row r="6" spans="1:16" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -1308,304 +1384,304 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="21">
         <v>7.0439999999999996</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="22">
         <v>7.9950000000000001</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="22">
         <v>6.931</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="22">
         <v>7.06</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="22">
         <v>7.2720000000000002</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="22">
         <v>6.8959999999999999</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="22">
         <v>6.8949999999999996</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="22">
         <v>6.9210000000000003</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="22">
         <v>6.9080000000000004</v>
       </c>
-      <c r="M7" s="36">
+      <c r="M7" s="23">
         <v>6.9039999999999999</v>
       </c>
-      <c r="N7" s="32">
+      <c r="N7" s="19">
         <f>AVERAGE(D7:M7)</f>
         <v>7.0826000000000011</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="20">
         <f>_xlfn.STDEV.P(D7:M7)</f>
         <v>0.32432089047731727</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
       <c r="N8" s="5"/>
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="21">
         <v>11.837999999999999</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="22">
         <v>11.848000000000001</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="22">
         <v>11.871</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="22">
         <v>11.864000000000001</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="22">
         <v>11.896000000000001</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="22">
         <v>11.862</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="22">
         <v>12.066000000000001</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="22">
         <v>11.862</v>
       </c>
-      <c r="L9" s="35">
+      <c r="L9" s="22">
         <v>11.993</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="23">
         <v>11.848000000000001</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="19">
         <f>AVERAGE(D9:M9)</f>
         <v>11.8948</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="20">
         <f>_xlfn.STDEV.P(D9:M9)</f>
         <v>7.0871432890834224E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="8"/>
       <c r="C10" s="3"/>
       <c r="N10" s="5"/>
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="21">
         <v>23.922999999999998</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="22">
         <v>24.341999999999999</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="22">
         <v>23.664999999999999</v>
       </c>
-      <c r="G11" s="35">
+      <c r="G11" s="22">
         <v>23.283000000000001</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="22">
         <v>23.872</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="22">
         <v>24.117000000000001</v>
       </c>
-      <c r="J11" s="35">
+      <c r="J11" s="22">
         <v>23.370999999999999</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="22">
         <v>23.402999999999999</v>
       </c>
-      <c r="L11" s="35">
+      <c r="L11" s="22">
         <v>23.484999999999999</v>
       </c>
-      <c r="M11" s="36">
+      <c r="M11" s="23">
         <v>23.315000000000001</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="19">
         <f>AVERAGE(D11:M11)</f>
         <v>23.677600000000002</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="20">
         <f>_xlfn.STDEV.P(D11:M11)</f>
         <v>0.35019457448681268</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="4"/>
       <c r="N12" s="5"/>
       <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="32" t="e">
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="19" t="e">
         <f>AVERAGE(D13:M13)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O13" s="33" t="e">
+      <c r="O13" s="20" t="e">
         <f>_xlfn.STDEV.P(D13:M13)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="15"/>
     </row>
     <row r="15" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="32" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="21">
         <v>16.052</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="22">
         <v>16.074000000000002</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="22">
         <v>16.097000000000001</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="22">
         <v>16.177</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H15" s="22">
         <v>16.239000000000001</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I15" s="22">
         <v>16.385000000000002</v>
       </c>
-      <c r="J15" s="35">
+      <c r="J15" s="22">
         <v>16.492000000000001</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="22">
         <v>16.466000000000001</v>
       </c>
-      <c r="L15" s="35">
+      <c r="L15" s="22">
         <v>16.463000000000001</v>
       </c>
-      <c r="M15" s="36">
+      <c r="M15" s="23">
         <v>16.146999999999998</v>
       </c>
-      <c r="N15" s="32">
+      <c r="N15" s="19">
         <f>AVERAGE(D15:M15)</f>
         <v>16.2592</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="20">
         <f>_xlfn.STDEV.P(D15:M15)</f>
         <v>0.16661800622981934</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="15"/>
     </row>
     <row r="17" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="21">
         <v>26.113</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="22">
         <v>26.268999999999998</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="22">
         <v>26.06</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="22">
         <v>26.161999999999999</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="22">
         <v>26.027999999999999</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="22">
         <v>26.274999999999999</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="22">
         <v>26.003</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="22">
         <v>26.11</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="22">
         <v>26.007000000000001</v>
       </c>
-      <c r="M17" s="36">
+      <c r="M17" s="23">
         <v>26.007999999999999</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="19">
         <f>AVERAGE(D17:M17)</f>
         <v>26.103499999999997</v>
       </c>
-      <c r="O17" s="33">
+      <c r="O17" s="20">
         <f>_xlfn.STDEV.P(D17:M17)</f>
         <v>9.8225505852603798E-2</v>
       </c>
@@ -1617,311 +1693,742 @@
       <c r="O18" s="15"/>
     </row>
     <row r="19" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="32" t="e">
+      <c r="D19" s="21">
+        <v>4.7119999999999997</v>
+      </c>
+      <c r="E19" s="22">
+        <v>4.6829999999999998</v>
+      </c>
+      <c r="F19" s="22">
+        <v>4.6760000000000002</v>
+      </c>
+      <c r="G19" s="22">
+        <v>4.6870000000000003</v>
+      </c>
+      <c r="H19" s="22">
+        <v>4.68</v>
+      </c>
+      <c r="I19" s="22">
+        <v>4.718</v>
+      </c>
+      <c r="J19" s="22">
+        <v>4.7359999999999998</v>
+      </c>
+      <c r="K19" s="22">
+        <v>4.6710000000000003</v>
+      </c>
+      <c r="L19" s="22">
+        <v>4.7</v>
+      </c>
+      <c r="M19" s="23">
+        <v>4.6790000000000003</v>
+      </c>
+      <c r="N19" s="19">
         <f>AVERAGE(D19:M19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O19" s="33" t="e">
+        <v>4.6942000000000004</v>
+      </c>
+      <c r="O19" s="20">
         <f>_xlfn.STDEV.P(D19:M19)</f>
-        <v>#DIV/0!</v>
+        <v>2.0355834544424738E-2</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="6"/>
       <c r="N20" s="5"/>
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="16" t="s">
+      <c r="A21" s="30"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="32" t="e">
+      <c r="D21" s="21">
+        <v>9.1739999999999995</v>
+      </c>
+      <c r="E21" s="22">
+        <v>9.1920000000000002</v>
+      </c>
+      <c r="F21" s="22">
+        <v>8.7739999999999991</v>
+      </c>
+      <c r="G21" s="22">
+        <v>9.2629999999999999</v>
+      </c>
+      <c r="H21" s="22">
+        <v>9.6140000000000008</v>
+      </c>
+      <c r="I21" s="22">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="J21" s="22">
+        <v>9.2929999999999993</v>
+      </c>
+      <c r="K21" s="22">
+        <v>9.2430000000000003</v>
+      </c>
+      <c r="L21" s="22">
+        <v>9.6020000000000003</v>
+      </c>
+      <c r="M21" s="23">
+        <v>9.1950000000000003</v>
+      </c>
+      <c r="N21" s="19">
         <f>AVERAGE(D21:M21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O21" s="33" t="e">
+        <v>9.2629999999999999</v>
+      </c>
+      <c r="O21" s="20">
         <f>_xlfn.STDEV.P(D21:M21)</f>
-        <v>#DIV/0!</v>
+        <v>0.2228043985203168</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8"/>
       <c r="C22" s="3"/>
       <c r="N22" s="5"/>
       <c r="O22" s="15"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="30"/>
+      <c r="B23" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="32" t="e">
+      <c r="D23" s="21">
+        <v>15.432</v>
+      </c>
+      <c r="E23" s="22">
+        <v>14.706</v>
+      </c>
+      <c r="F23" s="22">
+        <v>14.832000000000001</v>
+      </c>
+      <c r="G23" s="22">
+        <v>14.7</v>
+      </c>
+      <c r="H23" s="22">
+        <v>14.885</v>
+      </c>
+      <c r="I23" s="22">
+        <v>14.803000000000001</v>
+      </c>
+      <c r="J23" s="22">
+        <v>14.823</v>
+      </c>
+      <c r="K23" s="22">
+        <v>15.545999999999999</v>
+      </c>
+      <c r="L23" s="22">
+        <v>14.895</v>
+      </c>
+      <c r="M23" s="23">
+        <v>14.896000000000001</v>
+      </c>
+      <c r="N23" s="19">
         <f>AVERAGE(D23:M23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O23" s="33" t="e">
+        <v>14.951800000000002</v>
+      </c>
+      <c r="O23" s="20">
         <f>_xlfn.STDEV.P(D23:M23)</f>
-        <v>#DIV/0!</v>
+        <v>0.27773577371307417</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="6"/>
       <c r="N24" s="5"/>
       <c r="O24" s="15"/>
     </row>
     <row r="25" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="32" t="e">
+      <c r="D25" s="21">
+        <v>33.948999999999998</v>
+      </c>
+      <c r="E25" s="22">
+        <v>33.741999999999997</v>
+      </c>
+      <c r="F25" s="22">
+        <v>33.737000000000002</v>
+      </c>
+      <c r="G25" s="22">
+        <v>33.720999999999997</v>
+      </c>
+      <c r="H25" s="22">
+        <v>33.720999999999997</v>
+      </c>
+      <c r="I25" s="22">
+        <v>33.707000000000001</v>
+      </c>
+      <c r="J25" s="22">
+        <v>33.576999999999998</v>
+      </c>
+      <c r="K25" s="22">
+        <v>33.756</v>
+      </c>
+      <c r="L25" s="22">
+        <v>33.783000000000001</v>
+      </c>
+      <c r="M25" s="23">
+        <v>33.938000000000002</v>
+      </c>
+      <c r="N25" s="19">
         <f>AVERAGE(D25:M25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="33" t="e">
+        <v>33.763099999999994</v>
+      </c>
+      <c r="O25" s="20">
         <f>_xlfn.STDEV.P(D25:M25)</f>
-        <v>#DIV/0!</v>
+        <v>0.10394561077794548</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
       <c r="N26" s="5"/>
       <c r="O26" s="15"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="32" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="32" t="e">
+      <c r="D27" s="21">
+        <v>9.6189999999999998</v>
+      </c>
+      <c r="E27" s="22">
+        <v>9.0259999999999998</v>
+      </c>
+      <c r="F27" s="22">
+        <v>8.923</v>
+      </c>
+      <c r="G27" s="22">
+        <v>9.9480000000000004</v>
+      </c>
+      <c r="H27" s="22">
+        <v>8.6809999999999992</v>
+      </c>
+      <c r="I27" s="22">
+        <v>8.7669999999999995</v>
+      </c>
+      <c r="J27" s="22">
+        <v>9.7590000000000003</v>
+      </c>
+      <c r="K27" s="22">
+        <v>8.8889999999999993</v>
+      </c>
+      <c r="L27" s="22">
+        <v>9.8510000000000009</v>
+      </c>
+      <c r="M27" s="23">
+        <v>10.042999999999999</v>
+      </c>
+      <c r="N27" s="19">
         <f>AVERAGE(D27:M27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="33" t="e">
+        <v>9.3506</v>
+      </c>
+      <c r="O27" s="20">
         <f>_xlfn.STDEV.P(D27:M27)</f>
-        <v>#DIV/0!</v>
+        <v>0.51144583290901913</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="6"/>
       <c r="N28" s="5"/>
       <c r="O28" s="15"/>
     </row>
     <row r="29" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="34"/>
       <c r="C29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="32" t="e">
+      <c r="D29" s="21">
+        <v>19.827000000000002</v>
+      </c>
+      <c r="E29" s="22">
+        <v>18.138999999999999</v>
+      </c>
+      <c r="F29" s="22">
+        <v>18.016999999999999</v>
+      </c>
+      <c r="G29" s="22">
+        <v>18.242999999999999</v>
+      </c>
+      <c r="H29" s="22">
+        <v>18.166</v>
+      </c>
+      <c r="I29" s="22">
+        <v>18.099</v>
+      </c>
+      <c r="J29" s="22">
+        <v>18.052</v>
+      </c>
+      <c r="K29" s="22">
+        <v>18.201000000000001</v>
+      </c>
+      <c r="L29" s="22">
+        <v>18.404</v>
+      </c>
+      <c r="M29" s="23">
+        <v>18.841000000000001</v>
+      </c>
+      <c r="N29" s="19">
         <f>AVERAGE(D29:M29)</f>
+        <v>18.398900000000001</v>
+      </c>
+      <c r="O29" s="20">
+        <f>_xlfn.STDEV.P(D29:M29)</f>
+        <v>0.52690937550967976</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="18" t="e">
+        <f>AVERAGE(D31:M31)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O29" s="33" t="e">
-        <f>_xlfn.STDEV.P(D29:M29)</f>
+      <c r="O31" s="20" t="e">
+        <f>_xlfn.STDEV.P(D31:M31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30"/>
-    </row>
-    <row r="31" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31"/>
-    </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32"/>
-      <c r="C32" s="44"/>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33"/>
-      <c r="C33" s="44"/>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34"/>
-      <c r="C34" s="44"/>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35"/>
-      <c r="C35" s="44"/>
-    </row>
-    <row r="36" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36"/>
-      <c r="C36" s="44"/>
-    </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37"/>
-      <c r="C37" s="44"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38"/>
-      <c r="C38" s="44"/>
-    </row>
-    <row r="39" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39"/>
-      <c r="C39" s="44"/>
-    </row>
-    <row r="40" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40"/>
-      <c r="C40" s="44"/>
-    </row>
-    <row r="41" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41"/>
-      <c r="C41" s="44"/>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="30"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="11"/>
+    </row>
+    <row r="33" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="30"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="21">
+        <v>25.431000000000001</v>
+      </c>
+      <c r="E33" s="22">
+        <v>26.291</v>
+      </c>
+      <c r="F33" s="22">
+        <v>24.774999999999999</v>
+      </c>
+      <c r="G33" s="22">
+        <v>24.841000000000001</v>
+      </c>
+      <c r="H33" s="22">
+        <v>25.289000000000001</v>
+      </c>
+      <c r="I33" s="22">
+        <v>24.972000000000001</v>
+      </c>
+      <c r="J33" s="22">
+        <v>26.545999999999999</v>
+      </c>
+      <c r="K33" s="22">
+        <v>25.369</v>
+      </c>
+      <c r="L33" s="22">
+        <v>24.876000000000001</v>
+      </c>
+      <c r="M33" s="23">
+        <v>24.989000000000001</v>
+      </c>
+      <c r="N33" s="19">
+        <f>AVERAGE(D33:M33)</f>
+        <v>25.337899999999998</v>
+      </c>
+      <c r="O33" s="20">
+        <f>_xlfn.STDEV.P(D33:M33)</f>
+        <v>0.58418001506384976</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="30"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="15"/>
+    </row>
+    <row r="35" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="30"/>
+      <c r="B35" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="40"/>
+      <c r="N35" s="18" t="e">
+        <f>AVERAGE(D35:M35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" s="20" t="e">
+        <f>_xlfn.STDEV.P(D35:M35)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="30"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="15"/>
+    </row>
+    <row r="37" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="21">
+        <v>51.136000000000003</v>
+      </c>
+      <c r="E37" s="22">
+        <v>51.066000000000003</v>
+      </c>
+      <c r="F37" s="22">
+        <v>51.238</v>
+      </c>
+      <c r="G37" s="22">
+        <v>51.456000000000003</v>
+      </c>
+      <c r="H37" s="22">
+        <v>51.106000000000002</v>
+      </c>
+      <c r="I37" s="22">
+        <v>51.280999999999999</v>
+      </c>
+      <c r="J37" s="22">
+        <v>51.213999999999999</v>
+      </c>
+      <c r="K37" s="22">
+        <v>51.442</v>
+      </c>
+      <c r="L37" s="22">
+        <v>51.494999999999997</v>
+      </c>
+      <c r="M37" s="23">
+        <v>51.439</v>
+      </c>
+      <c r="N37" s="19">
+        <f>AVERAGE(D37:M37)</f>
+        <v>51.287300000000002</v>
+      </c>
+      <c r="O37" s="20">
+        <f>_xlfn.STDEV.P(D37:M37)</f>
+        <v>0.15202700418017773</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="30"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="15"/>
+    </row>
+    <row r="39" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="30"/>
+      <c r="B39" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="21">
+        <v>9.9269999999999996</v>
+      </c>
+      <c r="E39" s="22">
+        <v>8.7449999999999992</v>
+      </c>
+      <c r="F39" s="22">
+        <v>8.7959999999999994</v>
+      </c>
+      <c r="G39" s="22">
+        <v>9.7249999999999996</v>
+      </c>
+      <c r="H39" s="22">
+        <v>9.4570000000000007</v>
+      </c>
+      <c r="I39" s="22">
+        <v>9.8550000000000004</v>
+      </c>
+      <c r="J39" s="22">
+        <v>9.7219999999999995</v>
+      </c>
+      <c r="K39" s="22">
+        <v>8.5630000000000006</v>
+      </c>
+      <c r="L39" s="22">
+        <v>9.8249999999999993</v>
+      </c>
+      <c r="M39" s="23"/>
+      <c r="N39" s="19">
+        <f>AVERAGE(D39:M39)</f>
+        <v>9.4016666666666655</v>
+      </c>
+      <c r="O39" s="20">
+        <f>_xlfn.STDEV.P(D39:M39)</f>
+        <v>0.51341146591533504</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="30"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="15"/>
+    </row>
+    <row r="41" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="31"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="21">
+        <v>18.582000000000001</v>
+      </c>
+      <c r="E41" s="22">
+        <v>18.602</v>
+      </c>
+      <c r="F41" s="22">
+        <v>18.687999999999999</v>
+      </c>
+      <c r="G41" s="22">
+        <v>18.635000000000002</v>
+      </c>
+      <c r="H41" s="22">
+        <v>18.783000000000001</v>
+      </c>
+      <c r="I41" s="22">
+        <v>19.248000000000001</v>
+      </c>
+      <c r="J41" s="22">
+        <v>18.722000000000001</v>
+      </c>
+      <c r="K41" s="22">
+        <v>18.641999999999999</v>
+      </c>
+      <c r="L41" s="22">
+        <v>19.41</v>
+      </c>
+      <c r="M41" s="23"/>
+      <c r="N41" s="19">
+        <f>AVERAGE(D41:M41)</f>
+        <v>18.812444444444445</v>
+      </c>
+      <c r="O41" s="20">
+        <f>_xlfn.STDEV.P(D41:M41)</f>
+        <v>0.28465265816863394</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42"/>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44"/>
-    </row>
-    <row r="45" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45"/>
-    </row>
-    <row r="46" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46"/>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48"/>
-    </row>
-    <row r="49" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49"/>
-    </row>
-    <row r="50" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50"/>
-    </row>
-    <row r="51" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51"/>
-    </row>
-    <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52"/>
-    </row>
-    <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53"/>
-    </row>
-    <row r="54" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="48"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="55"/>
+    </row>
+    <row r="45" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="55"/>
+    </row>
+    <row r="46" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="48"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="55"/>
+    </row>
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="48"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="55"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="48"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="55"/>
+    </row>
+    <row r="49" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="47"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="55"/>
+    </row>
+    <row r="50" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="48"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="55"/>
+    </row>
+    <row r="51" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="48"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="55"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="48"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="55"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="48"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="54"/>
+    </row>
+    <row r="54" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54"/>
-    </row>
-    <row r="55" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="56"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="51"/>
+    </row>
+    <row r="55" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55"/>
-    </row>
-    <row r="56" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="56"/>
+      <c r="D55" s="51"/>
+    </row>
+    <row r="56" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56"/>
     </row>
-    <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64"/>
     </row>
     <row r="65" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2153,17 +2660,21 @@
       <c r="A140"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A7:A17"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D5:O5"/>
+    <mergeCell ref="A31:A41"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B39:B41"/>
     <mergeCell ref="A19:A29"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A7:A17"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:N6">
     <cfRule type="duplicateValues" dxfId="1" priority="3"/>
@@ -2180,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2192,14 +2703,14 @@
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:5" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
@@ -2214,13 +2725,13 @@
       <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -2231,960 +2742,1032 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="19">
         <v>7.0826000000000011</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="20">
         <v>0.32432089047731727</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="19">
         <v>11.8948</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="20">
         <v>7.0871432890834224E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="8"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="19">
         <v>23.677600000000002</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="20">
         <v>0.35019457448681268</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="6"/>
       <c r="D11" s="5"/>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="32" t="e">
+      <c r="D12" s="19" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E12" s="33" t="e">
+      <c r="E12" s="20" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="9"/>
       <c r="C13" s="6"/>
       <c r="D13" s="5"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="32" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="19">
         <v>16.2592</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="20">
         <v>0.16661800622981934</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="6"/>
       <c r="D15" s="5"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="19">
         <v>26.103499999999997</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="20">
         <v>9.8225505852603798E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="43"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="5"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="33" t="e">
-        <v>#DIV/0!</v>
+      <c r="D18" s="19">
+        <v>4.6942000000000004</v>
+      </c>
+      <c r="E18" s="20">
+        <v>2.0355834544424738E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="5"/>
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="33" t="e">
-        <v>#DIV/0!</v>
+      <c r="D20" s="19">
+        <v>9.2629999999999999</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0.2228043985203168</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="8"/>
       <c r="C21" s="3"/>
       <c r="D21" s="5"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="21" t="s">
+      <c r="A22" s="30"/>
+      <c r="B22" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" s="33" t="e">
-        <v>#DIV/0!</v>
+      <c r="D22" s="19">
+        <v>14.951800000000002</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0.27773577371307417</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="6"/>
       <c r="D23" s="5"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="33" t="e">
-        <v>#DIV/0!</v>
+      <c r="D24" s="19">
+        <v>33.763099999999994</v>
+      </c>
+      <c r="E24" s="20">
+        <v>0.10394561077794548</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
       <c r="D25" s="5"/>
       <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19"/>
-      <c r="B26" s="21" t="s">
+      <c r="A26" s="30"/>
+      <c r="B26" s="32" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="32" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="33" t="e">
-        <v>#DIV/0!</v>
+      <c r="D26" s="19">
+        <v>9.3506</v>
+      </c>
+      <c r="E26" s="20">
+        <v>0.51144583290901913</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="6"/>
       <c r="D27" s="5"/>
       <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="20"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="32" t="e">
+      <c r="D28" s="20">
+        <v>18.398900000000001</v>
+      </c>
+      <c r="E28" s="20">
+        <v>0.52690937550967976</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="20" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="E28" s="33" t="e">
+      <c r="E30" s="20" t="e">
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="43"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="43"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-    </row>
-    <row r="32" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-    </row>
-    <row r="33" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="43"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-    </row>
-    <row r="37" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-    </row>
-    <row r="38" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-    </row>
-    <row r="39" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-    </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-    </row>
-    <row r="42" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-    </row>
-    <row r="43" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-    </row>
-    <row r="44" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-    </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-    </row>
-    <row r="47" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="43"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-    </row>
-    <row r="48" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="43"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
+    <row r="31" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="30"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="30"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="19">
+        <v>25.337899999999998</v>
+      </c>
+      <c r="E32" s="20">
+        <v>0.58418001506384976</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="30"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="30"/>
+      <c r="B34" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="19" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E34" s="20" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="30"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="30"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="19">
+        <v>51.287300000000002</v>
+      </c>
+      <c r="E36" s="20">
+        <v>0.15202700418017773</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="30"/>
+      <c r="B38" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="19">
+        <v>9.4016666666666655</v>
+      </c>
+      <c r="E38" s="20">
+        <v>0.51341146591533504</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="30"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="31"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="19">
+        <v>18.812444444444445</v>
+      </c>
+      <c r="E40" s="20">
+        <v>0.28465265816863394</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+    </row>
+    <row r="42" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+    </row>
+    <row r="43" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+    </row>
+    <row r="44" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+    </row>
+    <row r="47" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+    </row>
+    <row r="48" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
     </row>
     <row r="49" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="43"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="43"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="43"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
     </row>
     <row r="52" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="43"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
     </row>
     <row r="53" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="43"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
     </row>
     <row r="54" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="43"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
     </row>
     <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="43"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="43"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
     </row>
     <row r="57" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
     </row>
     <row r="58" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="43"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
     </row>
     <row r="59" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="43"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="43"/>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="43"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
     </row>
     <row r="62" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="43"/>
-      <c r="B62" s="43"/>
-      <c r="C62" s="43"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
     </row>
     <row r="63" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="43"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
     </row>
     <row r="64" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="43"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
     </row>
     <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="43"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="43"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
+      <c r="A66" s="28"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
     </row>
     <row r="67" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="43"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
     </row>
     <row r="68" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="43"/>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
     </row>
     <row r="69" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="43"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="43"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="43"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="43"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="43"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="43"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
     </row>
     <row r="72" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="43"/>
-      <c r="B72" s="43"/>
-      <c r="C72" s="43"/>
+      <c r="A72" s="28"/>
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
     </row>
     <row r="73" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="43"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="43"/>
+      <c r="A73" s="28"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
     </row>
     <row r="74" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="43"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="43"/>
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="43"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
+      <c r="A75" s="28"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="43"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="43"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
     </row>
     <row r="77" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="43"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="43"/>
+      <c r="A77" s="28"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
     </row>
     <row r="78" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="43"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="43"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="28"/>
+      <c r="C78" s="28"/>
     </row>
     <row r="79" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="43"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="43"/>
+      <c r="A79" s="28"/>
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
     </row>
     <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="43"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="43"/>
+      <c r="A80" s="28"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="43"/>
-      <c r="B81" s="43"/>
-      <c r="C81" s="43"/>
+      <c r="A81" s="28"/>
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
     </row>
     <row r="82" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="43"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
+      <c r="A82" s="28"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="28"/>
     </row>
     <row r="83" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="43"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
     </row>
     <row r="84" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="43"/>
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
+      <c r="A84" s="28"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="43"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="43"/>
+      <c r="A85" s="28"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="43"/>
-      <c r="B86" s="43"/>
-      <c r="C86" s="43"/>
+      <c r="A86" s="28"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
     </row>
     <row r="87" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="43"/>
-      <c r="B87" s="43"/>
-      <c r="C87" s="43"/>
+      <c r="A87" s="28"/>
+      <c r="B87" s="28"/>
+      <c r="C87" s="28"/>
     </row>
     <row r="88" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="43"/>
-      <c r="B88" s="43"/>
-      <c r="C88" s="43"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
     </row>
     <row r="89" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="43"/>
-      <c r="B89" s="43"/>
-      <c r="C89" s="43"/>
+      <c r="A89" s="28"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="43"/>
-      <c r="B90" s="43"/>
-      <c r="C90" s="43"/>
+      <c r="A90" s="28"/>
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="43"/>
-      <c r="B91" s="43"/>
-      <c r="C91" s="43"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="28"/>
+      <c r="C91" s="28"/>
     </row>
     <row r="92" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="43"/>
-      <c r="B92" s="43"/>
-      <c r="C92" s="43"/>
+      <c r="A92" s="28"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="28"/>
     </row>
     <row r="93" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="43"/>
-      <c r="B93" s="43"/>
-      <c r="C93" s="43"/>
+      <c r="A93" s="28"/>
+      <c r="B93" s="28"/>
+      <c r="C93" s="28"/>
     </row>
     <row r="94" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="43"/>
-      <c r="B94" s="43"/>
-      <c r="C94" s="43"/>
+      <c r="A94" s="28"/>
+      <c r="B94" s="28"/>
+      <c r="C94" s="28"/>
     </row>
     <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="43"/>
-      <c r="B95" s="43"/>
-      <c r="C95" s="43"/>
+      <c r="A95" s="28"/>
+      <c r="B95" s="28"/>
+      <c r="C95" s="28"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="43"/>
-      <c r="B96" s="43"/>
-      <c r="C96" s="43"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
     </row>
     <row r="97" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="43"/>
-      <c r="B97" s="43"/>
-      <c r="C97" s="43"/>
+      <c r="A97" s="28"/>
+      <c r="B97" s="28"/>
+      <c r="C97" s="28"/>
     </row>
     <row r="98" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="43"/>
-      <c r="B98" s="43"/>
-      <c r="C98" s="43"/>
+      <c r="A98" s="28"/>
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
     </row>
     <row r="99" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="43"/>
-      <c r="B99" s="43"/>
-      <c r="C99" s="43"/>
+      <c r="A99" s="28"/>
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="43"/>
-      <c r="B100" s="43"/>
-      <c r="C100" s="43"/>
+      <c r="A100" s="28"/>
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="43"/>
-      <c r="B101" s="43"/>
-      <c r="C101" s="43"/>
+      <c r="A101" s="28"/>
+      <c r="B101" s="28"/>
+      <c r="C101" s="28"/>
     </row>
     <row r="102" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="43"/>
-      <c r="B102" s="43"/>
-      <c r="C102" s="43"/>
+      <c r="A102" s="28"/>
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
     </row>
     <row r="103" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="43"/>
-      <c r="B103" s="43"/>
-      <c r="C103" s="43"/>
+      <c r="A103" s="28"/>
+      <c r="B103" s="28"/>
+      <c r="C103" s="28"/>
     </row>
     <row r="104" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="43"/>
-      <c r="B104" s="43"/>
-      <c r="C104" s="43"/>
+      <c r="A104" s="28"/>
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
     </row>
     <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="43"/>
-      <c r="B105" s="43"/>
-      <c r="C105" s="43"/>
+      <c r="A105" s="28"/>
+      <c r="B105" s="28"/>
+      <c r="C105" s="28"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="43"/>
-      <c r="B106" s="43"/>
-      <c r="C106" s="43"/>
+      <c r="A106" s="28"/>
+      <c r="B106" s="28"/>
+      <c r="C106" s="28"/>
     </row>
     <row r="107" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="43"/>
-      <c r="B107" s="43"/>
-      <c r="C107" s="43"/>
+      <c r="A107" s="28"/>
+      <c r="B107" s="28"/>
+      <c r="C107" s="28"/>
     </row>
     <row r="108" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="43"/>
-      <c r="B108" s="43"/>
-      <c r="C108" s="43"/>
+      <c r="A108" s="28"/>
+      <c r="B108" s="28"/>
+      <c r="C108" s="28"/>
     </row>
     <row r="109" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="43"/>
-      <c r="B109" s="43"/>
-      <c r="C109" s="43"/>
+      <c r="A109" s="28"/>
+      <c r="B109" s="28"/>
+      <c r="C109" s="28"/>
     </row>
     <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="43"/>
-      <c r="B110" s="43"/>
-      <c r="C110" s="43"/>
+      <c r="A110" s="28"/>
+      <c r="B110" s="28"/>
+      <c r="C110" s="28"/>
     </row>
     <row r="111" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="43"/>
-      <c r="B111" s="43"/>
-      <c r="C111" s="43"/>
+      <c r="A111" s="28"/>
+      <c r="B111" s="28"/>
+      <c r="C111" s="28"/>
     </row>
     <row r="112" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="43"/>
-      <c r="B112" s="43"/>
-      <c r="C112" s="43"/>
+      <c r="A112" s="28"/>
+      <c r="B112" s="28"/>
+      <c r="C112" s="28"/>
     </row>
     <row r="113" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="43"/>
-      <c r="B113" s="43"/>
-      <c r="C113" s="43"/>
+      <c r="A113" s="28"/>
+      <c r="B113" s="28"/>
+      <c r="C113" s="28"/>
     </row>
     <row r="114" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="43"/>
-      <c r="B114" s="43"/>
-      <c r="C114" s="43"/>
+      <c r="A114" s="28"/>
+      <c r="B114" s="28"/>
+      <c r="C114" s="28"/>
     </row>
     <row r="115" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="43"/>
-      <c r="B115" s="43"/>
-      <c r="C115" s="43"/>
+      <c r="A115" s="28"/>
+      <c r="B115" s="28"/>
+      <c r="C115" s="28"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="43"/>
-      <c r="B116" s="43"/>
-      <c r="C116" s="43"/>
+      <c r="A116" s="28"/>
+      <c r="B116" s="28"/>
+      <c r="C116" s="28"/>
     </row>
     <row r="117" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="43"/>
-      <c r="B117" s="43"/>
-      <c r="C117" s="43"/>
+      <c r="A117" s="28"/>
+      <c r="B117" s="28"/>
+      <c r="C117" s="28"/>
     </row>
     <row r="118" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="43"/>
-      <c r="B118" s="43"/>
-      <c r="C118" s="43"/>
+      <c r="A118" s="28"/>
+      <c r="B118" s="28"/>
+      <c r="C118" s="28"/>
     </row>
     <row r="119" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="43"/>
-      <c r="B119" s="43"/>
-      <c r="C119" s="43"/>
+      <c r="A119" s="28"/>
+      <c r="B119" s="28"/>
+      <c r="C119" s="28"/>
     </row>
     <row r="120" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="43"/>
-      <c r="B120" s="43"/>
-      <c r="C120" s="43"/>
+      <c r="A120" s="28"/>
+      <c r="B120" s="28"/>
+      <c r="C120" s="28"/>
     </row>
     <row r="121" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="43"/>
-      <c r="B121" s="43"/>
-      <c r="C121" s="43"/>
+      <c r="A121" s="28"/>
+      <c r="B121" s="28"/>
+      <c r="C121" s="28"/>
     </row>
     <row r="122" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="43"/>
-      <c r="B122" s="43"/>
-      <c r="C122" s="43"/>
+      <c r="A122" s="28"/>
+      <c r="B122" s="28"/>
+      <c r="C122" s="28"/>
     </row>
     <row r="123" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="43"/>
-      <c r="B123" s="43"/>
-      <c r="C123" s="43"/>
+      <c r="A123" s="28"/>
+      <c r="B123" s="28"/>
+      <c r="C123" s="28"/>
     </row>
     <row r="124" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="43"/>
-      <c r="B124" s="43"/>
-      <c r="C124" s="43"/>
+      <c r="A124" s="28"/>
+      <c r="B124" s="28"/>
+      <c r="C124" s="28"/>
     </row>
     <row r="125" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="43"/>
-      <c r="B125" s="43"/>
-      <c r="C125" s="43"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="28"/>
+      <c r="C125" s="28"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="43"/>
-      <c r="B126" s="43"/>
-      <c r="C126" s="43"/>
+      <c r="A126" s="28"/>
+      <c r="B126" s="28"/>
+      <c r="C126" s="28"/>
     </row>
     <row r="127" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="43"/>
-      <c r="B127" s="43"/>
-      <c r="C127" s="43"/>
+      <c r="A127" s="28"/>
+      <c r="B127" s="28"/>
+      <c r="C127" s="28"/>
     </row>
     <row r="128" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="43"/>
-      <c r="B128" s="43"/>
-      <c r="C128" s="43"/>
+      <c r="A128" s="28"/>
+      <c r="B128" s="28"/>
+      <c r="C128" s="28"/>
     </row>
     <row r="129" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="43"/>
-      <c r="B129" s="43"/>
-      <c r="C129" s="43"/>
+      <c r="A129" s="28"/>
+      <c r="B129" s="28"/>
+      <c r="C129" s="28"/>
     </row>
     <row r="130" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="43"/>
-      <c r="B130" s="43"/>
-      <c r="C130" s="43"/>
+      <c r="A130" s="28"/>
+      <c r="B130" s="28"/>
+      <c r="C130" s="28"/>
     </row>
     <row r="131" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="43"/>
-      <c r="B131" s="43"/>
-      <c r="C131" s="43"/>
+      <c r="A131" s="28"/>
+      <c r="B131" s="28"/>
+      <c r="C131" s="28"/>
     </row>
     <row r="132" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="43"/>
-      <c r="B132" s="43"/>
-      <c r="C132" s="43"/>
+      <c r="A132" s="28"/>
+      <c r="B132" s="28"/>
+      <c r="C132" s="28"/>
     </row>
     <row r="133" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="43"/>
-      <c r="B133" s="43"/>
-      <c r="C133" s="43"/>
+      <c r="A133" s="28"/>
+      <c r="B133" s="28"/>
+      <c r="C133" s="28"/>
     </row>
     <row r="134" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="43"/>
-      <c r="B134" s="43"/>
-      <c r="C134" s="43"/>
+      <c r="A134" s="28"/>
+      <c r="B134" s="28"/>
+      <c r="C134" s="28"/>
     </row>
     <row r="135" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="43"/>
-      <c r="B135" s="43"/>
-      <c r="C135" s="43"/>
+      <c r="A135" s="28"/>
+      <c r="B135" s="28"/>
+      <c r="C135" s="28"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="43"/>
-      <c r="B136" s="43"/>
-      <c r="C136" s="43"/>
+      <c r="A136" s="28"/>
+      <c r="B136" s="28"/>
+      <c r="C136" s="28"/>
     </row>
     <row r="137" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="43"/>
-      <c r="B137" s="43"/>
-      <c r="C137" s="43"/>
+      <c r="A137" s="28"/>
+      <c r="B137" s="28"/>
+      <c r="C137" s="28"/>
     </row>
     <row r="138" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="43"/>
-      <c r="B138" s="43"/>
-      <c r="C138" s="43"/>
+      <c r="A138" s="28"/>
+      <c r="B138" s="28"/>
+      <c r="C138" s="28"/>
     </row>
     <row r="139" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="43"/>
-      <c r="B139" s="43"/>
-      <c r="C139" s="43"/>
+      <c r="A139" s="28"/>
+      <c r="B139" s="28"/>
+      <c r="C139" s="28"/>
     </row>
     <row r="140" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="43"/>
-      <c r="B140" s="43"/>
-      <c r="C140" s="43"/>
+      <c r="A140" s="28"/>
+      <c r="B140" s="28"/>
+      <c r="C140" s="28"/>
     </row>
     <row r="141" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="43"/>
-      <c r="B141" s="43"/>
-      <c r="C141" s="43"/>
+      <c r="A141" s="28"/>
+      <c r="B141" s="28"/>
+      <c r="C141" s="28"/>
     </row>
     <row r="142" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="43"/>
-      <c r="B142" s="43"/>
-      <c r="C142" s="43"/>
+      <c r="A142" s="28"/>
+      <c r="B142" s="28"/>
+      <c r="C142" s="28"/>
     </row>
     <row r="143" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="43"/>
-      <c r="B143" s="43"/>
-      <c r="C143" s="43"/>
+      <c r="A143" s="28"/>
+      <c r="B143" s="28"/>
+      <c r="C143" s="28"/>
     </row>
     <row r="144" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="43"/>
-      <c r="B144" s="43"/>
-      <c r="C144" s="43"/>
+      <c r="A144" s="28"/>
+      <c r="B144" s="28"/>
+      <c r="C144" s="28"/>
     </row>
     <row r="145" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="43"/>
-      <c r="B145" s="43"/>
-      <c r="C145" s="43"/>
+      <c r="A145" s="28"/>
+      <c r="B145" s="28"/>
+      <c r="C145" s="28"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="43"/>
-      <c r="B146" s="43"/>
-      <c r="C146" s="43"/>
+      <c r="A146" s="28"/>
+      <c r="B146" s="28"/>
+      <c r="C146" s="28"/>
     </row>
     <row r="147" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="43"/>
-      <c r="B147" s="43"/>
-      <c r="C147" s="43"/>
+      <c r="A147" s="28"/>
+      <c r="B147" s="28"/>
+      <c r="C147" s="28"/>
     </row>
     <row r="148" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="43"/>
-      <c r="B148" s="43"/>
-      <c r="C148" s="43"/>
+      <c r="A148" s="28"/>
+      <c r="B148" s="28"/>
+      <c r="C148" s="28"/>
     </row>
     <row r="149" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="43"/>
-      <c r="B149" s="43"/>
-      <c r="C149" s="43"/>
+      <c r="A149" s="28"/>
+      <c r="B149" s="28"/>
+      <c r="C149" s="28"/>
     </row>
     <row r="150" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="43"/>
-      <c r="B150" s="43"/>
-      <c r="C150" s="43"/>
+      <c r="A150" s="28"/>
+      <c r="B150" s="28"/>
+      <c r="C150" s="28"/>
     </row>
     <row r="151" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="43"/>
-      <c r="B151" s="43"/>
-      <c r="C151" s="43"/>
+      <c r="A151" s="28"/>
+      <c r="B151" s="28"/>
+      <c r="C151" s="28"/>
     </row>
     <row r="152" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="43"/>
-      <c r="B152" s="43"/>
-      <c r="C152" s="43"/>
+      <c r="A152" s="28"/>
+      <c r="B152" s="28"/>
+      <c r="C152" s="28"/>
     </row>
     <row r="153" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="43"/>
-      <c r="B153" s="43"/>
-      <c r="C153" s="43"/>
+      <c r="A153" s="28"/>
+      <c r="B153" s="28"/>
+      <c r="C153" s="28"/>
     </row>
     <row r="154" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="43"/>
-      <c r="B154" s="43"/>
-      <c r="C154" s="43"/>
+      <c r="A154" s="28"/>
+      <c r="B154" s="28"/>
+      <c r="C154" s="28"/>
     </row>
     <row r="155" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="43"/>
-      <c r="B155" s="43"/>
-      <c r="C155" s="43"/>
+      <c r="A155" s="28"/>
+      <c r="B155" s="28"/>
+      <c r="C155" s="28"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="43"/>
-      <c r="B156" s="43"/>
-      <c r="C156" s="43"/>
+      <c r="A156" s="28"/>
+      <c r="B156" s="28"/>
+      <c r="C156" s="28"/>
     </row>
     <row r="157" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="43"/>
-      <c r="B157" s="43"/>
-      <c r="C157" s="43"/>
+      <c r="A157" s="28"/>
+      <c r="B157" s="28"/>
+      <c r="C157" s="28"/>
     </row>
     <row r="158" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="43"/>
-      <c r="B158" s="43"/>
-      <c r="C158" s="43"/>
+      <c r="A158" s="28"/>
+      <c r="B158" s="28"/>
+      <c r="C158" s="28"/>
     </row>
     <row r="159" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="43"/>
-      <c r="B159" s="43"/>
-      <c r="C159" s="43"/>
+      <c r="A159" s="28"/>
+      <c r="B159" s="28"/>
+      <c r="C159" s="28"/>
     </row>
     <row r="160" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="43"/>
-      <c r="B160" s="43"/>
-      <c r="C160" s="43"/>
+      <c r="A160" s="28"/>
+      <c r="B160" s="28"/>
+      <c r="C160" s="28"/>
     </row>
     <row r="161" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="43"/>
-      <c r="B161" s="43"/>
-      <c r="C161" s="43"/>
+      <c r="A161" s="28"/>
+      <c r="B161" s="28"/>
+      <c r="C161" s="28"/>
     </row>
     <row r="162" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="43"/>
-      <c r="B162" s="43"/>
-      <c r="C162" s="43"/>
+      <c r="A162" s="28"/>
+      <c r="B162" s="28"/>
+      <c r="C162" s="28"/>
     </row>
     <row r="163" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="43"/>
-      <c r="B163" s="43"/>
-      <c r="C163" s="43"/>
+      <c r="A163" s="28"/>
+      <c r="B163" s="28"/>
+      <c r="C163" s="28"/>
     </row>
     <row r="164" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="43"/>
-      <c r="B164" s="43"/>
-      <c r="C164" s="43"/>
+      <c r="A164" s="28"/>
+      <c r="B164" s="28"/>
+      <c r="C164" s="28"/>
     </row>
     <row r="165" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="43"/>
-      <c r="B165" s="43"/>
-      <c r="C165" s="43"/>
+      <c r="A165" s="28"/>
+      <c r="B165" s="28"/>
+      <c r="C165" s="28"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="43"/>
-      <c r="B166" s="43"/>
-      <c r="C166" s="43"/>
+      <c r="A166" s="28"/>
+      <c r="B166" s="28"/>
+      <c r="C166" s="28"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="43"/>
-      <c r="B167" s="43"/>
-      <c r="C167" s="43"/>
+      <c r="A167" s="28"/>
+      <c r="B167" s="28"/>
+      <c r="C167" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="A18:A28"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A30:A40"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B38:B40"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:A16"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A18:A28"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <conditionalFormatting sqref="D5">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
@@ -3195,14 +3778,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC1D6F7-562F-4B01-ACDE-32CE1A0B8072}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="39"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="46"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:U3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Report half done at methodology
</commit_message>
<xml_diff>
--- a/AllResults_Table - runs.xlsx
+++ b/AllResults_Table - runs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="40">
   <si>
     <t>ALL RESULTS</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Erato.</t>
+  </si>
+  <si>
+    <t>Home only</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1065,6 +1068,11 @@
     </xf>
     <xf numFmtId="165" fontId="26" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1104,6 +1112,39 @@
     <xf numFmtId="0" fontId="22" fillId="29" borderId="20" xfId="38" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,44 +1163,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1212,17 +1218,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1352,7 +1348,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Quick comparison'!$C$4:$C$8</c:f>
+              <c:f>'Quick comparison'!$C$5:$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1518,7 +1514,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Quick comparison'!$D$4:$D$7</c:f>
+              <c:f>'Quick comparison'!$D$5:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1539,7 +1535,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Quick comparison'!$E$4:$E$7</c:f>
+              <c:f>'Quick comparison'!$E$5:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1570,7 +1566,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Quick comparison'!$C$10:$C$14</c:f>
+              <c:f>'Quick comparison'!$C$11:$C$15</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1736,7 +1732,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Quick comparison'!$D$10:$D$13</c:f>
+              <c:f>'Quick comparison'!$D$11:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1757,7 +1753,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Quick comparison'!$E$10:$E$13</c:f>
+              <c:f>'Quick comparison'!$E$11:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1788,7 +1784,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Quick comparison'!$C$16:$C$20</c:f>
+              <c:f>'Quick comparison'!$C$17:$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1954,7 +1950,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'Quick comparison'!$D$16:$D$19</c:f>
+              <c:f>'Quick comparison'!$D$17:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1975,7 +1971,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Quick comparison'!$E$16:$E$19</c:f>
+              <c:f>'Quick comparison'!$E$17:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3452,7 +3448,6 @@
         <c:crossAx val="510678392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10000000"/>
         <c:minorUnit val="100000"/>
       </c:valAx>
       <c:valAx>
@@ -4062,7 +4057,6 @@
         <c:crossAx val="510678392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10000000"/>
         <c:minorUnit val="100000"/>
       </c:valAx>
       <c:valAx>
@@ -4672,7 +4666,7 @@
         <c:crossAx val="510678392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10000000"/>
+        <c:majorUnit val="20000000"/>
         <c:minorUnit val="100000"/>
       </c:valAx>
       <c:valAx>
@@ -6101,7 +6095,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25.337899999999998</c:v>
+                  <c:v>12.229699999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>51.287300000000002</c:v>
@@ -10841,7 +10835,7 @@
   <dimension ref="A1:AF140"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:N41"/>
+      <selection activeCell="O7" sqref="O7:O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10862,92 +10856,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="62" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="65"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="70"/>
     </row>
     <row r="5" spans="1:32" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
     </row>
     <row r="6" spans="1:32" s="62" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="95" t="s">
+      <c r="I6" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="95" t="s">
+      <c r="J6" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="95" t="s">
+      <c r="K6" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="95" t="s">
+      <c r="L6" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="95" t="s">
+      <c r="M6" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="96" t="s">
+      <c r="N6" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="96" t="s">
+      <c r="O6" s="66" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -10993,8 +10987,8 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="70"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="2"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
@@ -11010,8 +11004,8 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:32" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
@@ -11055,7 +11049,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1"/>
       <c r="N10" s="3"/>
@@ -11077,8 +11071,8 @@
       <c r="AF10" s="62"/>
     </row>
     <row r="11" spans="1:32" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="69" t="s">
+      <c r="A11" s="72"/>
+      <c r="B11" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -11124,15 +11118,15 @@
       </c>
     </row>
     <row r="12" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="2"/>
       <c r="N12" s="3"/>
       <c r="O12" s="12"/>
     </row>
     <row r="13" spans="1:32" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
-      <c r="B13" s="71"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="13" t="s">
         <v>13</v>
       </c>
@@ -11176,15 +11170,15 @@
       </c>
     </row>
     <row r="14" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="7"/>
       <c r="C14" s="2"/>
       <c r="N14" s="3"/>
       <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:32" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="69" t="s">
+      <c r="A15" s="72"/>
+      <c r="B15" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -11230,15 +11224,15 @@
       </c>
     </row>
     <row r="16" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="70"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="2"/>
       <c r="N16" s="3"/>
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -11288,10 +11282,10 @@
       <c r="O18" s="12"/>
     </row>
     <row r="19" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -11337,15 +11331,15 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
-      <c r="B20" s="70"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="4"/>
       <c r="N20" s="3"/>
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="71"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="76"/>
       <c r="C21" s="13" t="s">
         <v>13</v>
       </c>
@@ -11389,15 +11383,15 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1"/>
       <c r="N22" s="3"/>
       <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="69" t="s">
+      <c r="A23" s="72"/>
+      <c r="B23" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -11443,15 +11437,15 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="70"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="4"/>
       <c r="N24" s="3"/>
       <c r="O24" s="12"/>
     </row>
     <row r="25" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="71"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="13" t="s">
         <v>13</v>
       </c>
@@ -11495,15 +11489,15 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="N26" s="3"/>
       <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="69" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -11549,15 +11543,15 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="70"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="4"/>
       <c r="N28" s="3"/>
       <c r="O28" s="12"/>
     </row>
     <row r="29" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
-      <c r="B29" s="71"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="13" t="s">
         <v>13</v>
       </c>
@@ -11602,19 +11596,19 @@
     </row>
     <row r="30" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
-      <c r="N30" s="97"/>
+      <c r="N30" s="67"/>
     </row>
     <row r="31" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="93">
+      <c r="D31" s="63">
         <v>6.3079999999999998</v>
       </c>
       <c r="E31" s="8">
@@ -11641,7 +11635,7 @@
       <c r="L31" s="8">
         <v>6.3579999999999997</v>
       </c>
-      <c r="M31" s="94">
+      <c r="M31" s="64">
         <v>6.2530000000000001</v>
       </c>
       <c r="N31" s="14">
@@ -11654,8 +11648,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="70"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="4"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -11671,52 +11665,52 @@
       <c r="O32" s="9"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="67"/>
-      <c r="B33" s="71"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="76"/>
       <c r="C33" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="17">
-        <v>25.431000000000001</v>
-      </c>
-      <c r="E33" s="18">
-        <v>26.291</v>
-      </c>
-      <c r="F33" s="18">
-        <v>24.774999999999999</v>
-      </c>
-      <c r="G33" s="18">
-        <v>24.841000000000001</v>
-      </c>
-      <c r="H33" s="18">
-        <v>25.289000000000001</v>
-      </c>
-      <c r="I33" s="18">
-        <v>24.972000000000001</v>
-      </c>
-      <c r="J33" s="18">
-        <v>26.545999999999999</v>
-      </c>
-      <c r="K33" s="18">
-        <v>25.369</v>
-      </c>
-      <c r="L33" s="18">
-        <v>24.876000000000001</v>
-      </c>
-      <c r="M33" s="19">
-        <v>24.989000000000001</v>
+      <c r="D33" s="63">
+        <v>12.677</v>
+      </c>
+      <c r="E33" s="8">
+        <v>12.087999999999999</v>
+      </c>
+      <c r="F33" s="8">
+        <v>12.27</v>
+      </c>
+      <c r="G33" s="8">
+        <v>12.183999999999999</v>
+      </c>
+      <c r="H33" s="8">
+        <v>12.129</v>
+      </c>
+      <c r="I33" s="8">
+        <v>12.21</v>
+      </c>
+      <c r="J33" s="8">
+        <v>12.134</v>
+      </c>
+      <c r="K33" s="8">
+        <v>12.202999999999999</v>
+      </c>
+      <c r="L33" s="8">
+        <v>12.196</v>
+      </c>
+      <c r="M33" s="64">
+        <v>12.206</v>
       </c>
       <c r="N33" s="15">
         <f>AVERAGE(D33:M33)</f>
-        <v>25.337899999999998</v>
+        <v>12.229699999999999</v>
       </c>
       <c r="O33" s="16">
         <f>_xlfn.STDEV.P(D33:M33)</f>
-        <v>0.58418001506384976</v>
+        <v>0.15683306411595738</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="67"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1"/>
       <c r="D34" s="22"/>
@@ -11733,14 +11727,14 @@
       <c r="O34" s="12"/>
     </row>
     <row r="35" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="67"/>
-      <c r="B35" s="69" t="s">
+      <c r="A35" s="72"/>
+      <c r="B35" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="93">
+      <c r="D35" s="63">
         <v>21.516999999999999</v>
       </c>
       <c r="E35" s="8">
@@ -11767,7 +11761,7 @@
       <c r="L35" s="8">
         <v>29.210999999999999</v>
       </c>
-      <c r="M35" s="94">
+      <c r="M35" s="64">
         <v>25.991</v>
       </c>
       <c r="N35" s="14">
@@ -11780,8 +11774,8 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="67"/>
-      <c r="B36" s="70"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="4"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -11797,8 +11791,8 @@
       <c r="O36" s="12"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="67"/>
-      <c r="B37" s="71"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="13" t="s">
         <v>13</v>
       </c>
@@ -11842,7 +11836,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="67"/>
+      <c r="A38" s="72"/>
       <c r="B38" s="7"/>
       <c r="C38" s="4"/>
       <c r="D38" s="22"/>
@@ -11859,8 +11853,8 @@
       <c r="O38" s="12"/>
     </row>
     <row r="39" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="67"/>
-      <c r="B39" s="69" t="s">
+      <c r="A39" s="72"/>
+      <c r="B39" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C39" s="13" t="s">
@@ -11904,8 +11898,8 @@
       </c>
     </row>
     <row r="40" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="67"/>
-      <c r="B40" s="70"/>
+      <c r="A40" s="72"/>
+      <c r="B40" s="75"/>
       <c r="C40" s="4"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -11921,8 +11915,8 @@
       <c r="O40" s="12"/>
     </row>
     <row r="41" spans="1:15" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="68"/>
-      <c r="B41" s="71"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="76"/>
       <c r="C41" s="13" t="s">
         <v>13</v>
       </c>
@@ -12324,8 +12318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E168"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12337,13 +12331,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -12399,10 +12393,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -12416,15 +12410,15 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="70"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="4"/>
       <c r="D8" s="24"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
@@ -12436,15 +12430,15 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1"/>
       <c r="D10" s="24"/>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="69" t="s">
+      <c r="A11" s="72"/>
+      <c r="B11" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -12458,15 +12452,15 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="4"/>
       <c r="D12" s="24"/>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
-      <c r="B13" s="71"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="13" t="s">
         <v>13</v>
       </c>
@@ -12478,15 +12472,15 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="7"/>
       <c r="C14" s="4"/>
       <c r="D14" s="24"/>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="69" t="s">
+      <c r="A15" s="72"/>
+      <c r="B15" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -12500,15 +12494,15 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="70"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="4"/>
       <c r="D16" s="24"/>
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -12527,10 +12521,10 @@
       <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -12544,15 +12538,15 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
-      <c r="B20" s="70"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="4"/>
       <c r="D20" s="24"/>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="71"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="76"/>
       <c r="C21" s="13" t="s">
         <v>13</v>
       </c>
@@ -12564,15 +12558,15 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1"/>
       <c r="D22" s="24"/>
       <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="69" t="s">
+      <c r="A23" s="72"/>
+      <c r="B23" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="13" t="s">
@@ -12586,15 +12580,15 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="70"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="4"/>
       <c r="D24" s="24"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="71"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="13" t="s">
         <v>13</v>
       </c>
@@ -12606,15 +12600,15 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="24"/>
       <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="69" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -12628,15 +12622,15 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="70"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="4"/>
       <c r="D28" s="24"/>
       <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
-      <c r="B29" s="71"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="13" t="s">
         <v>13</v>
       </c>
@@ -12655,10 +12649,10 @@
       <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="13" t="s">
@@ -12672,35 +12666,35 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="70"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="4"/>
       <c r="D32" s="24"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="67"/>
-      <c r="B33" s="71"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="76"/>
       <c r="C33" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="16">
-        <v>25.337899999999998</v>
+        <v>12.229699999999999</v>
       </c>
       <c r="E33" s="16">
-        <v>0.58418001506384976</v>
+        <v>0.15683306411595738</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="67"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1"/>
       <c r="D34" s="24"/>
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="67"/>
-      <c r="B35" s="69" t="s">
+      <c r="A35" s="72"/>
+      <c r="B35" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -12714,15 +12708,15 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="67"/>
-      <c r="B36" s="70"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="4"/>
       <c r="D36" s="24"/>
       <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="67"/>
-      <c r="B37" s="71"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="13" t="s">
         <v>13</v>
       </c>
@@ -12734,15 +12728,15 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="67"/>
+      <c r="A38" s="72"/>
       <c r="B38" s="7"/>
       <c r="C38" s="4"/>
       <c r="D38" s="24"/>
       <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="67"/>
-      <c r="B39" s="69" t="s">
+      <c r="A39" s="72"/>
+      <c r="B39" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C39" s="13" t="s">
@@ -12756,15 +12750,15 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="67"/>
-      <c r="B40" s="70"/>
+      <c r="A40" s="72"/>
+      <c r="B40" s="75"/>
       <c r="C40" s="4"/>
       <c r="D40" s="24"/>
       <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="68"/>
-      <c r="B41" s="71"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="76"/>
       <c r="C41" s="13" t="s">
         <v>13</v>
       </c>
@@ -13412,6 +13406,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:A17"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="A19:A29"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B23:B25"/>
@@ -13420,11 +13419,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A7:A17"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
     <cfRule type="duplicateValues" dxfId="1" priority="4"/>
@@ -13435,10 +13429,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13449,7 +13443,7 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -13457,261 +13451,273 @@
       <c r="E1" s="49"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="98" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="98"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E4" s="35" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="42"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="66" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="73" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="36">
-        <v>100000</v>
-      </c>
-      <c r="E4" s="52">
-        <v>3.1E-4</v>
       </c>
       <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="24">
+      <c r="B5" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="36">
+        <v>100000</v>
+      </c>
+      <c r="E5" s="52">
+        <v>3.1E-4</v>
+      </c>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="24">
         <v>1000000</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E6" s="24">
         <v>3.2456E-3</v>
-      </c>
-      <c r="F5" s="42"/>
-    </row>
-    <row r="6" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="24">
-        <v>10000000</v>
-      </c>
-      <c r="E6" s="24">
-        <v>4.3196400000000003E-2</v>
       </c>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="24">
+        <v>10000000</v>
+      </c>
+      <c r="E7" s="24">
+        <v>4.3196400000000003E-2</v>
+      </c>
+      <c r="F7" s="42"/>
+    </row>
+    <row r="8" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="24">
         <v>100000000</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E8" s="24">
         <v>0.83599999999999997</v>
       </c>
-      <c r="F7" s="42"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="37">
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="37">
         <v>1000000000</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E9" s="38">
         <v>11.8948</v>
       </c>
-      <c r="F8" s="42"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
       <c r="F9" s="42"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="36">
-        <v>100000</v>
-      </c>
-      <c r="E10" s="36">
-        <v>5.7470000000000004E-4</v>
-      </c>
+      <c r="B10" s="72"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="24">
+      <c r="B11" s="72"/>
+      <c r="C11" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="36">
+        <v>100000</v>
+      </c>
+      <c r="E11" s="36">
+        <v>5.7470000000000004E-4</v>
+      </c>
+      <c r="F11" s="42"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="24">
         <v>1000000</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E12" s="52">
         <v>8.8503999999999996E-3</v>
-      </c>
-      <c r="F11" s="42"/>
-    </row>
-    <row r="12" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="24">
-        <v>10000000</v>
-      </c>
-      <c r="E12" s="24">
-        <v>0.21932489999999999</v>
       </c>
       <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="24">
+        <v>10000000</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.21932489999999999</v>
+      </c>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="24">
         <v>100000000</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E14" s="24">
         <v>3.294</v>
       </c>
-      <c r="F13" s="42"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="37">
+      <c r="F14" s="42"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="37">
         <v>1000000000</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E15" s="38">
         <v>52.392999999999994</v>
       </c>
-      <c r="F14" s="42"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
       <c r="F15" s="42"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="36">
-        <v>100000</v>
-      </c>
-      <c r="E16" s="36">
-        <v>6.4570000000000003E-4</v>
-      </c>
+      <c r="B16" s="72"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="24">
+      <c r="B17" s="72"/>
+      <c r="C17" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="36">
+        <v>100000</v>
+      </c>
+      <c r="E17" s="36">
+        <v>6.4570000000000003E-4</v>
+      </c>
+      <c r="F17" s="42"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="24">
         <v>1000000</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E18" s="24">
         <v>6.0870999999999998E-3</v>
-      </c>
-      <c r="F17" s="42"/>
-    </row>
-    <row r="18" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="24">
-        <v>10000000</v>
-      </c>
-      <c r="E18" s="24">
-        <v>7.2176299999999999E-2</v>
       </c>
       <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="74"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="24">
+        <v>10000000</v>
+      </c>
+      <c r="E19" s="24">
+        <v>7.2176299999999999E-2</v>
+      </c>
+      <c r="F19" s="42"/>
+    </row>
+    <row r="20" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="24">
         <v>100000000</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E20" s="24">
         <v>1.5469999999999999</v>
       </c>
-      <c r="F19" s="42"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="37">
+      <c r="F20" s="42"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="37">
         <v>1000000000</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E21" s="38">
         <v>26.103499999999997</v>
       </c>
-      <c r="F20" s="42"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
       <c r="F21" s="42"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="43"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="47"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="B4:B20"/>
+  <mergeCells count="5">
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="B5:B21"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="E4">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13719,8 +13725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Z101" sqref="Z101"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S128" sqref="S128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13734,52 +13740,52 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="89"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="83"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="90"/>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91"/>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="92"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="86"/>
     </row>
     <row r="29" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:22" x14ac:dyDescent="0.25">
@@ -14189,11 +14195,11 @@
       </c>
       <c r="F48" s="23"/>
       <c r="G48" s="23"/>
-      <c r="H48" s="85" t="s">
+      <c r="H48" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="87"/>
       <c r="K48" s="42"/>
       <c r="M48" s="3"/>
       <c r="N48" s="23" t="s">
@@ -14205,11 +14211,11 @@
       </c>
       <c r="Q48" s="23"/>
       <c r="R48" s="23"/>
-      <c r="S48" s="85" t="s">
+      <c r="S48" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="T48" s="85"/>
-      <c r="U48" s="85"/>
+      <c r="T48" s="87"/>
+      <c r="U48" s="87"/>
       <c r="V48" s="42"/>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
@@ -14223,12 +14229,12 @@
       </c>
       <c r="F49" s="23"/>
       <c r="G49" s="23"/>
-      <c r="H49" s="86">
+      <c r="H49" s="88">
         <f>CORREL(C49:C52,E49:E52)</f>
         <v>0.99899045759129523</v>
       </c>
-      <c r="I49" s="86"/>
-      <c r="J49" s="86"/>
+      <c r="I49" s="88"/>
+      <c r="J49" s="88"/>
       <c r="K49" s="42"/>
       <c r="M49" s="3"/>
       <c r="N49" s="23">
@@ -14240,12 +14246,12 @@
       </c>
       <c r="Q49" s="23"/>
       <c r="R49" s="23"/>
-      <c r="S49" s="86">
+      <c r="S49" s="88">
         <f>CORREL(N49:N52,P49:P52)</f>
         <v>0.99955105717609127</v>
       </c>
-      <c r="T49" s="86"/>
-      <c r="U49" s="86"/>
+      <c r="T49" s="88"/>
+      <c r="U49" s="88"/>
       <c r="V49" s="42"/>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.25">
@@ -14259,9 +14265,9 @@
       </c>
       <c r="F50" s="23"/>
       <c r="G50" s="23"/>
-      <c r="H50" s="86"/>
-      <c r="I50" s="86"/>
-      <c r="J50" s="86"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="88"/>
+      <c r="J50" s="88"/>
       <c r="K50" s="42"/>
       <c r="M50" s="3"/>
       <c r="N50" s="23">
@@ -14273,9 +14279,9 @@
       </c>
       <c r="Q50" s="23"/>
       <c r="R50" s="23"/>
-      <c r="S50" s="86"/>
-      <c r="T50" s="86"/>
-      <c r="U50" s="86"/>
+      <c r="S50" s="88"/>
+      <c r="T50" s="88"/>
+      <c r="U50" s="88"/>
       <c r="V50" s="42"/>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.25">
@@ -14588,11 +14594,11 @@
       </c>
       <c r="F73" s="23"/>
       <c r="G73" s="23"/>
-      <c r="H73" s="85" t="s">
+      <c r="H73" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="I73" s="85"/>
-      <c r="J73" s="85"/>
+      <c r="I73" s="87"/>
+      <c r="J73" s="87"/>
       <c r="K73" s="42"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -14606,12 +14612,12 @@
       </c>
       <c r="F74" s="23"/>
       <c r="G74" s="23"/>
-      <c r="H74" s="86">
+      <c r="H74" s="88">
         <f>CORREL(C74:C77,E74:E77)</f>
         <v>0.99875823505410932</v>
       </c>
-      <c r="I74" s="86"/>
-      <c r="J74" s="86"/>
+      <c r="I74" s="88"/>
+      <c r="J74" s="88"/>
       <c r="K74" s="42"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -14625,9 +14631,9 @@
       </c>
       <c r="F75" s="23"/>
       <c r="G75" s="23"/>
-      <c r="H75" s="86"/>
-      <c r="I75" s="86"/>
-      <c r="J75" s="86"/>
+      <c r="H75" s="88"/>
+      <c r="I75" s="88"/>
+      <c r="J75" s="88"/>
       <c r="K75" s="42"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -14676,52 +14682,52 @@
     </row>
     <row r="80" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="87" t="s">
+      <c r="A81" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="B81" s="88"/>
-      <c r="C81" s="88"/>
-      <c r="D81" s="88"/>
-      <c r="E81" s="88"/>
-      <c r="F81" s="88"/>
-      <c r="G81" s="88"/>
-      <c r="H81" s="88"/>
-      <c r="I81" s="88"/>
-      <c r="J81" s="88"/>
-      <c r="K81" s="88"/>
-      <c r="L81" s="88"/>
-      <c r="M81" s="88"/>
-      <c r="N81" s="88"/>
-      <c r="O81" s="88"/>
-      <c r="P81" s="88"/>
-      <c r="Q81" s="88"/>
-      <c r="R81" s="88"/>
-      <c r="S81" s="88"/>
-      <c r="T81" s="88"/>
-      <c r="U81" s="89"/>
+      <c r="B81" s="82"/>
+      <c r="C81" s="82"/>
+      <c r="D81" s="82"/>
+      <c r="E81" s="82"/>
+      <c r="F81" s="82"/>
+      <c r="G81" s="82"/>
+      <c r="H81" s="82"/>
+      <c r="I81" s="82"/>
+      <c r="J81" s="82"/>
+      <c r="K81" s="82"/>
+      <c r="L81" s="82"/>
+      <c r="M81" s="82"/>
+      <c r="N81" s="82"/>
+      <c r="O81" s="82"/>
+      <c r="P81" s="82"/>
+      <c r="Q81" s="82"/>
+      <c r="R81" s="82"/>
+      <c r="S81" s="82"/>
+      <c r="T81" s="82"/>
+      <c r="U81" s="83"/>
     </row>
     <row r="82" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="90"/>
-      <c r="B82" s="91"/>
-      <c r="C82" s="91"/>
-      <c r="D82" s="91"/>
-      <c r="E82" s="91"/>
-      <c r="F82" s="91"/>
-      <c r="G82" s="91"/>
-      <c r="H82" s="91"/>
-      <c r="I82" s="91"/>
-      <c r="J82" s="91"/>
-      <c r="K82" s="91"/>
-      <c r="L82" s="91"/>
-      <c r="M82" s="91"/>
-      <c r="N82" s="91"/>
-      <c r="O82" s="91"/>
-      <c r="P82" s="91"/>
-      <c r="Q82" s="91"/>
-      <c r="R82" s="91"/>
-      <c r="S82" s="91"/>
-      <c r="T82" s="91"/>
-      <c r="U82" s="92"/>
+      <c r="A82" s="84"/>
+      <c r="B82" s="85"/>
+      <c r="C82" s="85"/>
+      <c r="D82" s="85"/>
+      <c r="E82" s="85"/>
+      <c r="F82" s="85"/>
+      <c r="G82" s="85"/>
+      <c r="H82" s="85"/>
+      <c r="I82" s="85"/>
+      <c r="J82" s="85"/>
+      <c r="K82" s="85"/>
+      <c r="L82" s="85"/>
+      <c r="M82" s="85"/>
+      <c r="N82" s="85"/>
+      <c r="O82" s="85"/>
+      <c r="P82" s="85"/>
+      <c r="Q82" s="85"/>
+      <c r="R82" s="85"/>
+      <c r="S82" s="85"/>
+      <c r="T82" s="85"/>
+      <c r="U82" s="86"/>
     </row>
     <row r="83" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
@@ -14787,13 +14793,13 @@
       <c r="N86" s="23"/>
       <c r="O86" s="23"/>
       <c r="P86" s="23"/>
-      <c r="Q86" s="82" t="s">
+      <c r="Q86" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="R86" s="83"/>
-      <c r="S86" s="83"/>
-      <c r="T86" s="83"/>
-      <c r="U86" s="84"/>
+      <c r="R86" s="90"/>
+      <c r="S86" s="90"/>
+      <c r="T86" s="90"/>
+      <c r="U86" s="91"/>
     </row>
     <row r="87" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3"/>
@@ -14813,12 +14819,12 @@
       <c r="O87" s="23"/>
       <c r="P87" s="60"/>
       <c r="Q87" s="54"/>
-      <c r="R87" s="76" t="s">
+      <c r="R87" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="S87" s="77"/>
-      <c r="T87" s="77"/>
-      <c r="U87" s="78"/>
+      <c r="S87" s="93"/>
+      <c r="T87" s="93"/>
+      <c r="U87" s="94"/>
     </row>
     <row r="88" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3"/>
@@ -14837,7 +14843,7 @@
       <c r="N88" s="23"/>
       <c r="O88" s="23"/>
       <c r="P88" s="23"/>
-      <c r="Q88" s="79" t="s">
+      <c r="Q88" s="95" t="s">
         <v>32</v>
       </c>
       <c r="R88" s="58"/>
@@ -14868,7 +14874,7 @@
       <c r="N89" s="23"/>
       <c r="O89" s="23"/>
       <c r="P89" s="23"/>
-      <c r="Q89" s="80"/>
+      <c r="Q89" s="96"/>
       <c r="R89" s="59" t="s">
         <v>22</v>
       </c>
@@ -14902,7 +14908,7 @@
       <c r="N90" s="23"/>
       <c r="O90" s="23"/>
       <c r="P90" s="23"/>
-      <c r="Q90" s="81"/>
+      <c r="Q90" s="97"/>
       <c r="R90" s="50" t="s">
         <v>24</v>
       </c>
@@ -15005,13 +15011,13 @@
       <c r="N94" s="23"/>
       <c r="O94" s="23"/>
       <c r="P94" s="23"/>
-      <c r="Q94" s="82" t="s">
+      <c r="Q94" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="R94" s="83"/>
-      <c r="S94" s="83"/>
-      <c r="T94" s="83"/>
-      <c r="U94" s="84"/>
+      <c r="R94" s="90"/>
+      <c r="S94" s="90"/>
+      <c r="T94" s="90"/>
+      <c r="U94" s="91"/>
     </row>
     <row r="95" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3"/>
@@ -15031,12 +15037,12 @@
       <c r="O95" s="23"/>
       <c r="P95" s="23"/>
       <c r="Q95" s="54"/>
-      <c r="R95" s="76" t="s">
+      <c r="R95" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="S95" s="77"/>
-      <c r="T95" s="77"/>
-      <c r="U95" s="78"/>
+      <c r="S95" s="93"/>
+      <c r="T95" s="93"/>
+      <c r="U95" s="94"/>
     </row>
     <row r="96" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3"/>
@@ -15055,7 +15061,7 @@
       <c r="N96" s="23"/>
       <c r="O96" s="23"/>
       <c r="P96" s="23"/>
-      <c r="Q96" s="79" t="s">
+      <c r="Q96" s="95" t="s">
         <v>32</v>
       </c>
       <c r="R96" s="58"/>
@@ -15086,7 +15092,7 @@
       <c r="N97" s="23"/>
       <c r="O97" s="23"/>
       <c r="P97" s="23"/>
-      <c r="Q97" s="80"/>
+      <c r="Q97" s="96"/>
       <c r="R97" s="59" t="s">
         <v>22</v>
       </c>
@@ -15120,7 +15126,7 @@
       <c r="N98" s="23"/>
       <c r="O98" s="23"/>
       <c r="P98" s="23"/>
-      <c r="Q98" s="81"/>
+      <c r="Q98" s="97"/>
       <c r="R98" s="50" t="s">
         <v>24</v>
       </c>
@@ -15545,13 +15551,13 @@
       <c r="N116" s="23"/>
       <c r="O116" s="23"/>
       <c r="P116" s="23"/>
-      <c r="Q116" s="82" t="s">
+      <c r="Q116" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="R116" s="83"/>
-      <c r="S116" s="83"/>
-      <c r="T116" s="83"/>
-      <c r="U116" s="84"/>
+      <c r="R116" s="90"/>
+      <c r="S116" s="90"/>
+      <c r="T116" s="90"/>
+      <c r="U116" s="91"/>
     </row>
     <row r="117" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="3"/>
@@ -15571,12 +15577,12 @@
       <c r="O117" s="23"/>
       <c r="P117" s="60"/>
       <c r="Q117" s="54"/>
-      <c r="R117" s="76" t="s">
+      <c r="R117" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="S117" s="77"/>
-      <c r="T117" s="77"/>
-      <c r="U117" s="78"/>
+      <c r="S117" s="93"/>
+      <c r="T117" s="93"/>
+      <c r="U117" s="94"/>
     </row>
     <row r="118" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3"/>
@@ -15595,7 +15601,7 @@
       <c r="N118" s="23"/>
       <c r="O118" s="23"/>
       <c r="P118" s="23"/>
-      <c r="Q118" s="79" t="s">
+      <c r="Q118" s="95" t="s">
         <v>32</v>
       </c>
       <c r="R118" s="58"/>
@@ -15626,7 +15632,7 @@
       <c r="N119" s="23"/>
       <c r="O119" s="23"/>
       <c r="P119" s="23"/>
-      <c r="Q119" s="80"/>
+      <c r="Q119" s="96"/>
       <c r="R119" s="59" t="s">
         <v>22</v>
       </c>
@@ -15660,13 +15666,13 @@
       <c r="N120" s="23"/>
       <c r="O120" s="23"/>
       <c r="P120" s="23"/>
-      <c r="Q120" s="81"/>
+      <c r="Q120" s="97"/>
       <c r="R120" s="50" t="s">
         <v>24</v>
       </c>
       <c r="S120" s="61">
         <f>'Table of Results'!D9/'Table of Results'!D33</f>
-        <v>0.46944695495680389</v>
+        <v>0.97261584503299348</v>
       </c>
       <c r="T120" s="46">
         <f>'Table of Results'!D13/'Table of Results'!D37</f>
@@ -15763,13 +15769,13 @@
       <c r="N124" s="23"/>
       <c r="O124" s="23"/>
       <c r="P124" s="23"/>
-      <c r="Q124" s="82" t="s">
+      <c r="Q124" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="R124" s="83"/>
-      <c r="S124" s="83"/>
-      <c r="T124" s="83"/>
-      <c r="U124" s="84"/>
+      <c r="R124" s="90"/>
+      <c r="S124" s="90"/>
+      <c r="T124" s="90"/>
+      <c r="U124" s="91"/>
     </row>
     <row r="125" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="3"/>
@@ -15789,12 +15795,12 @@
       <c r="O125" s="23"/>
       <c r="P125" s="23"/>
       <c r="Q125" s="54"/>
-      <c r="R125" s="76" t="s">
+      <c r="R125" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="S125" s="77"/>
-      <c r="T125" s="77"/>
-      <c r="U125" s="78"/>
+      <c r="S125" s="93"/>
+      <c r="T125" s="93"/>
+      <c r="U125" s="94"/>
     </row>
     <row r="126" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="3"/>
@@ -15813,7 +15819,7 @@
       <c r="N126" s="23"/>
       <c r="O126" s="23"/>
       <c r="P126" s="23"/>
-      <c r="Q126" s="79" t="s">
+      <c r="Q126" s="95" t="s">
         <v>32</v>
       </c>
       <c r="R126" s="58"/>
@@ -15844,7 +15850,7 @@
       <c r="N127" s="23"/>
       <c r="O127" s="23"/>
       <c r="P127" s="23"/>
-      <c r="Q127" s="80"/>
+      <c r="Q127" s="96"/>
       <c r="R127" s="59" t="s">
         <v>22</v>
       </c>
@@ -15878,13 +15884,13 @@
       <c r="N128" s="23"/>
       <c r="O128" s="23"/>
       <c r="P128" s="23"/>
-      <c r="Q128" s="81"/>
+      <c r="Q128" s="97"/>
       <c r="R128" s="50" t="s">
         <v>24</v>
       </c>
       <c r="S128" s="61">
         <f t="shared" si="1"/>
-        <v>0.11736173873920097</v>
+        <v>0.24315396125824837</v>
       </c>
       <c r="T128" s="46">
         <f t="shared" si="1"/>
@@ -16242,26 +16248,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="R117:U117"/>
+    <mergeCell ref="Q118:Q120"/>
+    <mergeCell ref="Q124:U124"/>
+    <mergeCell ref="R125:U125"/>
+    <mergeCell ref="Q126:Q128"/>
+    <mergeCell ref="Q88:Q90"/>
+    <mergeCell ref="Q94:U94"/>
+    <mergeCell ref="R95:U95"/>
+    <mergeCell ref="Q96:Q98"/>
+    <mergeCell ref="Q116:U116"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="H74:J75"/>
+    <mergeCell ref="A81:U82"/>
+    <mergeCell ref="Q86:U86"/>
+    <mergeCell ref="R87:U87"/>
     <mergeCell ref="A2:U3"/>
     <mergeCell ref="H48:J48"/>
     <mergeCell ref="H49:J50"/>
     <mergeCell ref="S48:U48"/>
     <mergeCell ref="S49:U50"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="H74:J75"/>
-    <mergeCell ref="A81:U82"/>
-    <mergeCell ref="Q86:U86"/>
-    <mergeCell ref="R87:U87"/>
-    <mergeCell ref="Q88:Q90"/>
-    <mergeCell ref="Q94:U94"/>
-    <mergeCell ref="R95:U95"/>
-    <mergeCell ref="Q96:Q98"/>
-    <mergeCell ref="Q116:U116"/>
-    <mergeCell ref="R117:U117"/>
-    <mergeCell ref="Q118:Q120"/>
-    <mergeCell ref="Q124:U124"/>
-    <mergeCell ref="R125:U125"/>
-    <mergeCell ref="Q126:Q128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>